<commit_message>
feat: initial functions to define time betweenkeys
</commit_message>
<xml_diff>
--- a/Class/test.xlsx
+++ b/Class/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
   <si>
     <t>1-1</t>
   </si>
@@ -22,13 +22,394 @@
     <t>1-2</t>
   </si>
   <si>
+    <t>1-3</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>1-5</t>
+  </si>
+  <si>
+    <t>1-6</t>
+  </si>
+  <si>
+    <t>1-7</t>
+  </si>
+  <si>
+    <t>1-8</t>
+  </si>
+  <si>
+    <t>1-9</t>
+  </si>
+  <si>
+    <t>1-0</t>
+  </si>
+  <si>
+    <t>1-CONFIRMA</t>
+  </si>
+  <si>
+    <t>1-BRANCO</t>
+  </si>
+  <si>
+    <t>1-CORRIGE</t>
+  </si>
+  <si>
+    <t>2-1</t>
+  </si>
+  <si>
+    <t>2-2</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>2-4</t>
+  </si>
+  <si>
+    <t>2-5</t>
+  </si>
+  <si>
+    <t>2-6</t>
+  </si>
+  <si>
+    <t>2-7</t>
+  </si>
+  <si>
+    <t>2-8</t>
+  </si>
+  <si>
+    <t>2-9</t>
+  </si>
+  <si>
+    <t>2-0</t>
+  </si>
+  <si>
+    <t>2-CONFIRMA</t>
+  </si>
+  <si>
+    <t>2-BRANCO</t>
+  </si>
+  <si>
+    <t>2-CORRIGE</t>
+  </si>
+  <si>
+    <t>3-1</t>
+  </si>
+  <si>
+    <t>3-2</t>
+  </si>
+  <si>
+    <t>3-3</t>
+  </si>
+  <si>
+    <t>3-4</t>
+  </si>
+  <si>
+    <t>3-5</t>
+  </si>
+  <si>
+    <t>3-6</t>
+  </si>
+  <si>
+    <t>3-7</t>
+  </si>
+  <si>
+    <t>3-8</t>
+  </si>
+  <si>
+    <t>3-9</t>
+  </si>
+  <si>
+    <t>3-0</t>
+  </si>
+  <si>
+    <t>3-CONFIRMA</t>
+  </si>
+  <si>
+    <t>3-BRANCO</t>
+  </si>
+  <si>
+    <t>3-CORRIGE</t>
+  </si>
+  <si>
+    <t>4-1</t>
+  </si>
+  <si>
+    <t>4-2</t>
+  </si>
+  <si>
+    <t>4-3</t>
+  </si>
+  <si>
+    <t>4-4</t>
+  </si>
+  <si>
+    <t>4-5</t>
+  </si>
+  <si>
+    <t>4-6</t>
+  </si>
+  <si>
+    <t>4-7</t>
+  </si>
+  <si>
+    <t>4-8</t>
+  </si>
+  <si>
+    <t>4-9</t>
+  </si>
+  <si>
+    <t>4-0</t>
+  </si>
+  <si>
+    <t>4-CONFIRMA</t>
+  </si>
+  <si>
+    <t>4-BRANCO</t>
+  </si>
+  <si>
+    <t>4-CORRIGE</t>
+  </si>
+  <si>
+    <t>5-1</t>
+  </si>
+  <si>
+    <t>5-2</t>
+  </si>
+  <si>
+    <t>5-3</t>
+  </si>
+  <si>
+    <t>5-4</t>
+  </si>
+  <si>
+    <t>5-5</t>
+  </si>
+  <si>
+    <t>5-6</t>
+  </si>
+  <si>
+    <t>5-7</t>
+  </si>
+  <si>
+    <t>5-8</t>
+  </si>
+  <si>
+    <t>5-9</t>
+  </si>
+  <si>
+    <t>5-0</t>
+  </si>
+  <si>
+    <t>5-CONFIRMA</t>
+  </si>
+  <si>
+    <t>5-BRANCO</t>
+  </si>
+  <si>
+    <t>5-CORRIGE</t>
+  </si>
+  <si>
+    <t>6-1</t>
+  </si>
+  <si>
+    <t>6-2</t>
+  </si>
+  <si>
+    <t>6-3</t>
+  </si>
+  <si>
+    <t>6-4</t>
+  </si>
+  <si>
+    <t>6-5</t>
+  </si>
+  <si>
+    <t>6-6</t>
+  </si>
+  <si>
+    <t>6-7</t>
+  </si>
+  <si>
+    <t>6-8</t>
+  </si>
+  <si>
+    <t>6-9</t>
+  </si>
+  <si>
+    <t>6-0</t>
+  </si>
+  <si>
+    <t>6-CONFIRMA</t>
+  </si>
+  <si>
+    <t>6-BRANCO</t>
+  </si>
+  <si>
+    <t>6-CORRIGE</t>
+  </si>
+  <si>
+    <t>7-1</t>
+  </si>
+  <si>
+    <t>7-2</t>
+  </si>
+  <si>
+    <t>7-3</t>
+  </si>
+  <si>
+    <t>7-4</t>
+  </si>
+  <si>
+    <t>7-5</t>
+  </si>
+  <si>
+    <t>7-6</t>
+  </si>
+  <si>
+    <t>7-7</t>
+  </si>
+  <si>
+    <t>7-8</t>
+  </si>
+  <si>
+    <t>7-9</t>
+  </si>
+  <si>
+    <t>7-0</t>
+  </si>
+  <si>
+    <t>7-CONFIRMA</t>
+  </si>
+  <si>
+    <t>7-BRANCO</t>
+  </si>
+  <si>
+    <t>7-CORRIGE</t>
+  </si>
+  <si>
+    <t>8-1</t>
+  </si>
+  <si>
+    <t>8-2</t>
+  </si>
+  <si>
+    <t>8-3</t>
+  </si>
+  <si>
+    <t>8-4</t>
+  </si>
+  <si>
+    <t>8-5</t>
+  </si>
+  <si>
+    <t>8-6</t>
+  </si>
+  <si>
+    <t>8-7</t>
+  </si>
+  <si>
+    <t>8-8</t>
+  </si>
+  <si>
+    <t>8-9</t>
+  </si>
+  <si>
+    <t>8-0</t>
+  </si>
+  <si>
+    <t>8-CONFIRMA</t>
+  </si>
+  <si>
+    <t>8-BRANCO</t>
+  </si>
+  <si>
+    <t>8-CORRIGE</t>
+  </si>
+  <si>
+    <t>9-1</t>
+  </si>
+  <si>
+    <t>9-2</t>
+  </si>
+  <si>
+    <t>9-3</t>
+  </si>
+  <si>
+    <t>9-4</t>
+  </si>
+  <si>
+    <t>9-5</t>
+  </si>
+  <si>
+    <t>9-6</t>
+  </si>
+  <si>
+    <t>9-7</t>
+  </si>
+  <si>
+    <t>9-8</t>
+  </si>
+  <si>
+    <t>9-9</t>
+  </si>
+  <si>
+    <t>9-0</t>
+  </si>
+  <si>
+    <t>9-CONFIRMA</t>
+  </si>
+  <si>
+    <t>9-BRANCO</t>
+  </si>
+  <si>
+    <t>9-CORRIGE</t>
+  </si>
+  <si>
+    <t>0-1</t>
+  </si>
+  <si>
+    <t>0-2</t>
+  </si>
+  <si>
+    <t>0-3</t>
+  </si>
+  <si>
+    <t>0-4</t>
+  </si>
+  <si>
+    <t>0-5</t>
+  </si>
+  <si>
+    <t>0-6</t>
+  </si>
+  <si>
+    <t>0-7</t>
+  </si>
+  <si>
+    <t>0-8</t>
+  </si>
+  <si>
+    <t>0-9</t>
+  </si>
+  <si>
+    <t>0-0</t>
+  </si>
+  <si>
+    <t>0-CONFIRMA</t>
+  </si>
+  <si>
+    <t>0-BRANCO</t>
+  </si>
+  <si>
+    <t>0-CORRIGE</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
     <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
 </sst>
 </file>
@@ -386,45 +767,418 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:EA3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:131">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="CL1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CR1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CS1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CT1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CU1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CV1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CW1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CX1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CY1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="DB1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="DC1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="DD1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="DE1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="DH1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="DI1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="DM1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="DN1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="DO1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="DP1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="DR1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="DS1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="DU1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DV1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DW1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="DX1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="DY1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="DZ1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="EA1" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:131">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:131">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: implement list in dicts
and adjusts in compare digits
</commit_message>
<xml_diff>
--- a/Class/test.xlsx
+++ b/Class/test.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
+  <si>
+    <t>index</t>
+  </si>
   <si>
     <t>1-1</t>
   </si>
@@ -404,12 +407,6 @@
   </si>
   <si>
     <t>0-CORRIGE</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
 </sst>
 </file>
@@ -767,418 +764,1064 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:EA3"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:131">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="BX1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BY1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="BZ1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="CA1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="CB1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="CC1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="CD1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="CE1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="CF1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="CG1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="CH1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="CI1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="CJ1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="CK1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="CL1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="CM1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="CN1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="CO1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="CP1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="CQ1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="CR1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="CS1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="CT1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="CU1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="CV1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="CW1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="CX1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="CY1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="CZ1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="DA1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="DB1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="DC1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="DD1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="DE1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="DF1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="DG1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="DH1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="DI1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="DJ1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="DL1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="DM1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="DN1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="DO1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="DP1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="DQ1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="DR1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="DS1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="DT1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="DU1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="DV1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="DW1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="DX1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="DY1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="DZ1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="EA1" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:131">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:131">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="1">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="1">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="1">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="1">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="1">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="1">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="1">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="1">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="1">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="1">
+        <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="1">
+        <v>110</v>
+      </c>
+      <c r="B112" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="1">
+        <v>111</v>
+      </c>
+      <c r="B113" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="1">
+        <v>112</v>
+      </c>
+      <c r="B114" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="1">
+        <v>113</v>
+      </c>
+      <c r="B115" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="1">
+        <v>114</v>
+      </c>
+      <c r="B116" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="1">
+        <v>115</v>
+      </c>
+      <c r="B117" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="1">
+        <v>116</v>
+      </c>
+      <c r="B118" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="1">
+        <v>117</v>
+      </c>
+      <c r="B119" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="1">
+        <v>118</v>
+      </c>
+      <c r="B120" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="1">
+        <v>119</v>
+      </c>
+      <c r="B121" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="1">
+        <v>120</v>
+      </c>
+      <c r="B122" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="1">
+        <v>121</v>
+      </c>
+      <c r="B123" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="1">
+        <v>122</v>
+      </c>
+      <c r="B124" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="1">
+        <v>123</v>
+      </c>
+      <c r="B125" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="1">
+        <v>124</v>
+      </c>
+      <c r="B126" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="1">
+        <v>125</v>
+      </c>
+      <c r="B127" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="1">
+        <v>126</v>
+      </c>
+      <c r="B128" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="1">
+        <v>127</v>
+      </c>
+      <c r="B129" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="1">
+        <v>128</v>
+      </c>
+      <c r="B130" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="1">
+        <v>129</v>
+      </c>
+      <c r="B131" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>